<commit_message>
Actualizacion 9 marzo 2025
</commit_message>
<xml_diff>
--- a/PDF/data/educacion.xlsx
+++ b/PDF/data/educacion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Moni_HV\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monic\Documents\HV\PDF\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6155734D-6D42-4E50-A9D0-AD23B7319325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A0AF22-45AB-4E74-B750-CC0B1E0FEFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -64,9 +64,6 @@
     <t>Madrid, España</t>
   </si>
   <si>
-    <t xml:space="preserve">Maestría en Igualdad de género en ámbito público y privado </t>
-  </si>
-  <si>
     <t>Doctorado en Investigación de Medios de Comunicación</t>
   </si>
   <si>
@@ -80,6 +77,9 @@
   </si>
   <si>
     <t>Tesis: \href{http://hdl.handle.net/10016/35862}{El tratamiento periodístico de la violencia sexual en contra de las mujeres en el marco del conflicto armado colombiano. Análisis de casos según el tipo de violencia, víctimas, victimarios y contextos}. \textit{Cum Laude} y mención Internacional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maestría en Igualdad de Género en Ámbito Público y Privado </t>
   </si>
 </sst>
 </file>
@@ -570,48 +570,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -627,9 +627,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -667,7 +667,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -773,7 +773,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -915,7 +915,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -926,19 +926,19 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="135.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="135.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -955,9 +955,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>2022</v>
@@ -969,27 +969,27 @@
         <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>14</v>
       </c>
       <c r="B3">
         <v>2017</v>
       </c>
       <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>

</xml_diff>